<commit_message>
stoich ideas in xlsx file
</commit_message>
<xml_diff>
--- a/dev-examples/2025-stoich/all_stoich.xlsx
+++ b/dev-examples/2025-stoich/all_stoich.xlsx
@@ -1,32 +1,227 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au594831\GitHub_repos\ABM\dev-examples\2025-stoich\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2A0439-CFBA-4C8F-AA7A-41EBE1CE1A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="State vars" sheetId="1" r:id="rId1"/>
+    <sheet name="Substrates and products" sheetId="2" r:id="rId2"/>
+    <sheet name="Biomass" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="48">
+  <si>
+    <t>xa</t>
+  </si>
+  <si>
+    <t>xa_aer</t>
+  </si>
+  <si>
+    <t>xa_bac</t>
+  </si>
+  <si>
+    <t>xa_dead</t>
+  </si>
+  <si>
+    <t>RFd</t>
+  </si>
+  <si>
+    <t>iNDF</t>
+  </si>
+  <si>
+    <t>ash</t>
+  </si>
+  <si>
+    <t>VSd</t>
+  </si>
+  <si>
+    <t>starch</t>
+  </si>
+  <si>
+    <t>CPs</t>
+  </si>
+  <si>
+    <t>CPf</t>
+  </si>
+  <si>
+    <t>Cfat</t>
+  </si>
+  <si>
+    <t>VFA</t>
+  </si>
+  <si>
+    <t>urea</t>
+  </si>
+  <si>
+    <t>TAN</t>
+  </si>
+  <si>
+    <t>sulfate</t>
+  </si>
+  <si>
+    <t>sulfide</t>
+  </si>
+  <si>
+    <t>NH3_emis_cum</t>
+  </si>
+  <si>
+    <t>N2O_emis_cum</t>
+  </si>
+  <si>
+    <t>CH4_emis_cum</t>
+  </si>
+  <si>
+    <t>CO2_emis_cum</t>
+  </si>
+  <si>
+    <t>COD_conv_cum</t>
+  </si>
+  <si>
+    <t>COD_conv_cum_meth</t>
+  </si>
+  <si>
+    <t>COD_conv_cum_respir</t>
+  </si>
+  <si>
+    <t>COD_conv_cum_sr</t>
+  </si>
+  <si>
+    <t>COD_load_cum</t>
+  </si>
+  <si>
+    <t>C_load_cum</t>
+  </si>
+  <si>
+    <t>N_load_cum</t>
+  </si>
+  <si>
+    <t>slurry_load_cum</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>slu</t>
+  </si>
+  <si>
+    <t>slurry_prod_rate</t>
+  </si>
+  <si>
+    <t>rut</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>%*%</t>
+  </si>
+  <si>
+    <t>Reaction rate vector RR</t>
+  </si>
+  <si>
+    <t>Reaction coef matrix RC</t>
+  </si>
+  <si>
+    <t>RR =</t>
+  </si>
+  <si>
+    <t>Subtrate mass vector SM</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hydrolysis rate vector </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Reaction derivative vector RD</t>
+  </si>
+  <si>
+    <t>Total derivative vector TD</t>
+  </si>
+  <si>
+    <t>Loading vector L</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +244,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +546,916 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="18" width="3.6640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D50235F-572B-47B9-B819-D6FF1CB42A0C}">
+  <dimension ref="A1:AG23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="11" width="3.44140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.44140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="3" customWidth="1"/>
+    <col min="15" max="17" width="3.44140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" style="3" customWidth="1"/>
+    <col min="19" max="20" width="3.44140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.44140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="3.44140625" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="3.21875" customWidth="1"/>
+    <col min="29" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="2.44140625" customWidth="1"/>
+    <col min="33" max="33" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="Y1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="U8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="N9" t="s">
+        <v>12</v>
+      </c>
+      <c r="U9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="N15" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="R19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>11</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="14:18" x14ac:dyDescent="0.3">
+      <c r="N23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2FD2E-641C-489B-BD2A-42EF8CD38938}">
+  <dimension ref="A1:AF20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="10" width="3.44140625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="3" customWidth="1"/>
+    <col min="14" max="16" width="3.44140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" style="3" customWidth="1"/>
+    <col min="18" max="19" width="3.44140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="3.44140625" customWidth="1"/>
+    <col min="24" max="24" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="3.21875" customWidth="1"/>
+    <col min="28" max="28" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="2.44140625" customWidth="1"/>
+    <col min="32" max="32" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="2"/>
+      <c r="X1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AF1" s="6"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="M2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3"/>
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M6"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M7"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="K9" s="4"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:32" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="M16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M18"/>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M20"/>
+      <c r="Q20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
combine xa and subs in xls stoich ideas
</commit_message>
<xml_diff>
--- a/dev-examples/2025-stoich/all_stoich.xlsx
+++ b/dev-examples/2025-stoich/all_stoich.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au594831\GitHub_repos\ABM\dev-examples\2025-stoich\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2A0439-CFBA-4C8F-AA7A-41EBE1CE1A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0DA279-BD05-4F40-A96D-C79C13C9B6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="State vars" sheetId="1" r:id="rId1"/>
     <sheet name="Substrates and products" sheetId="2" r:id="rId2"/>
-    <sheet name="Biomass" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="48">
   <si>
     <t>xa</t>
   </si>
@@ -751,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D50235F-572B-47B9-B819-D6FF1CB42A0C}">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N9"/>
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,9 +1139,6 @@
       <c r="I12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="U12" t="s">
         <v>35</v>
       </c>
@@ -1156,303 +1152,220 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N13" s="6" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13"/>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="N14"/>
+      <c r="U14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="U17"/>
+    </row>
+    <row r="18" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="U18"/>
+    </row>
+    <row r="19" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U19"/>
+    </row>
+    <row r="20" spans="14:21" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="R20" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="N14" t="s">
+    <row r="21" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
         <v>7</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="N15" t="s">
+    <row r="22" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
         <v>4</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="N16" t="s">
+    <row r="23" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
         <v>5</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N17" t="s">
+    <row r="24" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N18" t="s">
+    <row r="25" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
         <v>9</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N19" t="s">
+    <row r="26" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
         <v>10</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N20" t="s">
+    <row r="27" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
         <v>11</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="14:18" x14ac:dyDescent="0.3">
-      <c r="N23" s="7" t="s">
+    <row r="30" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="P30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="R30" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2FD2E-641C-489B-BD2A-42EF8CD38938}">
-  <dimension ref="A1:AF20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="10" width="3.44140625" style="3" customWidth="1"/>
-    <col min="11" max="12" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="3" customWidth="1"/>
-    <col min="14" max="16" width="3.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" style="3" customWidth="1"/>
-    <col min="18" max="19" width="3.44140625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.44140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="3.44140625" customWidth="1"/>
-    <col min="24" max="24" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="3.21875" customWidth="1"/>
-    <col min="28" max="28" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="2.44140625" customWidth="1"/>
-    <col min="32" max="32" width="8.88671875" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="2"/>
-      <c r="X1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AF1" s="6"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="M2"/>
-      <c r="T2"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3"/>
-      <c r="T3"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4"/>
-      <c r="T4"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5"/>
-      <c r="T5"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M6"/>
-      <c r="T6"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M7"/>
-      <c r="T7"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M8"/>
-      <c r="T8"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="K9" s="4"/>
-      <c r="T9"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="T10"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="T11"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="T12"/>
-    </row>
-    <row r="13" spans="1:32" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M13" s="6"/>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M14"/>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M15"/>
-      <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="M16"/>
-      <c r="Q16"/>
-    </row>
-    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M17"/>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M18"/>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M19"/>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
-      <c r="M20"/>
-      <c r="Q20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>